<commit_message>
region of canada fit added
</commit_message>
<xml_diff>
--- a/Data/Country Policy Data/Canada.XLSX
+++ b/Data/Country Policy Data/Canada.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\Documents\GitHub\COVID-Tracking-Biola-Summer\Data\Country Policy Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc69fb6fe41d80c0/Documents/GitHub/COVID-Tracking-Biola-Summer/Data/Country Policy Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C552954-E068-4156-A96A-37312031CC91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8C552954-E068-4156-A96A-37312031CC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4682F402-1FCD-40CD-A213-B8C06614D6C6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,9 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,7 +377,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,7 +400,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>43907</v>
       </c>
       <c r="B2" t="s">
@@ -407,7 +411,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>44141</v>
       </c>
       <c r="B3" t="s">
@@ -415,7 +419,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>43955</v>
       </c>
       <c r="B4" t="s">
@@ -430,5 +434,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>